<commit_message>
add queue insertion and remotion
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t xml:space="preserve">LISTA</t>
   </si>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">tempo</t>
   </si>
   <si>
-    <t xml:space="preserve">tamanho da pilha</t>
+    <t xml:space="preserve">quantidade de itens</t>
   </si>
   <si>
     <t xml:space="preserve">inserção</t>
@@ -151,7 +151,37 @@
     <t xml:space="preserve">24.282717s</t>
   </si>
   <si>
+    <t xml:space="preserve">2778.127197s</t>
+  </si>
+  <si>
     <t xml:space="preserve">FILA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000016s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000154s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001448s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.015238s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remoção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000001s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000002s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000644s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.006622s</t>
   </si>
 </sst>
 </file>
@@ -197,12 +227,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -245,7 +281,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,40 +290,52 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -328,7 +376,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -371,16 +419,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="46:46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.14"/>
@@ -417,328 +466,332 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="5" t="n">
         <v>7392637</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="5" t="n">
         <v>959364</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="5" t="n">
         <v>63</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="5" t="n">
         <v>6154926</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="5" t="n">
         <v>11439</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+    <row r="6" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="5" t="n">
         <v>8712632876135</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="5" t="n">
         <v>960001</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="5" t="n">
         <v>63</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="5" t="n">
         <v>960001</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="5" t="n">
         <v>980</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="5" t="n">
         <v>1001</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="5" t="n">
         <v>764839</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="5" t="n">
         <v>1001</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
+    <row r="11" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="5" t="n">
         <v>5524699</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="5" t="n">
         <v>8502271</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="5" t="n">
         <v>996</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="5" t="n">
         <v>195931</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="5" t="n">
         <v>953340</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="5" t="n">
         <v>4280311</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="5" t="n">
         <v>666666</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
+    <row r="16" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="5" t="n">
         <v>10000</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="5" t="n">
         <v>100000</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="5" t="n">
         <v>960000</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="6" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="21" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
@@ -747,174 +800,289 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="0"/>
+      <c r="D23" s="6"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="8" t="n">
+      <c r="C24" s="12" t="n">
         <v>1000</v>
       </c>
-      <c r="D24" s="0"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="8" t="n">
+      <c r="C25" s="12" t="n">
         <v>10000</v>
       </c>
-      <c r="D25" s="0"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="8" t="n">
+      <c r="C26" s="12" t="n">
         <v>100000</v>
       </c>
-      <c r="D26" s="0"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="8" t="n">
+      <c r="C27" s="12" t="n">
         <v>1000000</v>
       </c>
-      <c r="D27" s="0"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="8" t="n">
+      <c r="C28" s="12" t="n">
         <v>10000000</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="8" t="n">
+      <c r="C30" s="12" t="n">
         <v>1000</v>
       </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="8" t="n">
+      <c r="C31" s="12" t="n">
         <v>10000</v>
       </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="8" t="n">
+      <c r="C32" s="12" t="n">
         <v>100000</v>
       </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="0"/>
-      <c r="C33" s="8" t="n">
+      <c r="B33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="12" t="n">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
+      <c r="B37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="12" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11"/>
+      <c r="B38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="12" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11"/>
+      <c r="B39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="12" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11"/>
+      <c r="B40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="12" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="41" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="12" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="14"/>
+      <c r="B43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="12" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14"/>
+      <c r="B44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="12" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="14"/>
+      <c r="B45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="12" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="46" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A42:A45"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>